<commit_message>
[NguyenPT][Coding] Update model class implements Serializable Create MainController class
</commit_message>
<xml_diff>
--- a/Document/AlaProject_Estimation.xlsx
+++ b/Document/AlaProject_Estimation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="116">
   <si>
     <t>Nghiên cứu chức năng app haivl trên Android</t>
   </si>
@@ -540,7 +540,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -598,8 +598,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -615,20 +623,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1050,11 +1044,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="26.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="2:5">
       <c r="B2" s="12" t="s">
@@ -1620,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1637,11 +1631,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8">
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" s="18" t="s">
@@ -1748,7 +1742,9 @@
       <c r="G6" s="10">
         <v>41860</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="19">
@@ -2306,7 +2302,7 @@
       <c r="B38" s="20">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D38" s="9">
@@ -2323,7 +2319,7 @@
       <c r="B39" s="20">
         <v>5.2</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D39" s="9">
@@ -2341,7 +2337,7 @@
       <c r="B40" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="C40" s="30" t="s">
         <v>107</v>
       </c>
       <c r="D40" s="9">
@@ -2358,7 +2354,7 @@
       <c r="B41" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="30" t="s">
         <v>108</v>
       </c>
       <c r="D41" s="9">
@@ -2375,7 +2371,7 @@
       <c r="B42" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D42" s="9">
@@ -2494,38 +2490,38 @@
       <c r="H47" s="11"/>
     </row>
     <row r="48" spans="2:8">
-      <c r="B48" s="36">
+      <c r="B48" s="27">
         <v>7.1</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="37">
+      <c r="D48" s="28">
         <v>16</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E48" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="37"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="28"/>
     </row>
     <row r="49" spans="2:8" ht="30">
-      <c r="B49" s="36">
+      <c r="B49" s="27">
         <v>7.2</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="C49" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D49" s="37">
+      <c r="D49" s="28">
         <v>8</v>
       </c>
-      <c r="E49" s="37" t="s">
+      <c r="E49" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="37"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="28"/>
     </row>
     <row r="50" spans="2:8">
       <c r="B50" s="21">
@@ -2668,12 +2664,12 @@
       <c r="D56" s="3">
         <v>16</v>
       </c>
-      <c r="E56" s="33" t="s">
+      <c r="E56" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="35"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
     </row>
     <row r="57" spans="2:8">
       <c r="B57" s="20"/>
@@ -2684,10 +2680,10 @@
         <f>SUM(D3,D7,D10,D15,D36,D43,D50:D55)</f>
         <v>182</v>
       </c>
-      <c r="E57" s="30"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="32"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>